<commit_message>
add write data code
</commit_message>
<xml_diff>
--- a/src/com/SpiceTG/TestDataFiles/ForgotPwdUserName.xlsx
+++ b/src/com/SpiceTG/TestDataFiles/ForgotPwdUserName.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Empty</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -105,7 +105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -114,7 +114,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -426,68 +425,69 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>